<commit_message>
-implemnted a health system & UI system -implemnted crouching -fixed grounded
</commit_message>
<xml_diff>
--- a/Functionality Testing doc.xlsx
+++ b/Functionality Testing doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30007736\Desktop\Repos\3D Game Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71D1146A-0B2A-4F18-8FFB-00E4B2C42FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96742665-D6B6-42EB-B6DF-3D9BAC3AFBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0468E738-A089-472E-90BF-358012EA3B5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Test Case</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Returns a value of 100</t>
+  </si>
+  <si>
+    <t>health bar image fill changes in correspondance with the player's current health value when damge is received</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1AD350-2B3B-4B9B-B52A-E9E11B598E62}">
-  <dimension ref="B1:E6"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +604,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>